<commit_message>
More changes - particularly arduino code
</commit_message>
<xml_diff>
--- a/colour-theory/colour-palettes/colours.xlsx
+++ b/colour-theory/colour-palettes/colours.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/dr19500_bristol_ac_uk/Documents/Project 2020/Colour Palettes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/dr19500_bristol_ac_uk/Documents/Project 2020/colour-theory/colour-palettes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="143" documentId="8_{7C6CD7C7-0BCB-4184-B93E-C2276493D1ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4DF16B4C-3FFA-4826-BDDC-E5378BB10D7D}"/>
+  <xr:revisionPtr revIDLastSave="144" documentId="8_{7C6CD7C7-0BCB-4184-B93E-C2276493D1ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0A9988E4-A495-3440-B1CC-841BDFFD4E34}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-9660" yWindow="120" windowWidth="14500" windowHeight="9460" firstSheet="6" activeTab="6" xr2:uid="{E8E95DA0-770C-4812-975B-CF66929D1793}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{E8E95DA0-770C-4812-975B-CF66929D1793}"/>
   </bookViews>
   <sheets>
     <sheet name="Pleasure" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="316">
   <si>
     <t>Blue</t>
   </si>
@@ -1084,7 +1084,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1682,7 +1682,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3750,13 +3750,13 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -3764,7 +3764,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -3772,7 +3772,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -3780,7 +3780,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -3788,7 +3788,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -3796,7 +3796,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -3804,7 +3804,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -3812,7 +3812,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -3820,7 +3820,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -3828,7 +3828,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -3836,7 +3836,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -3854,17 +3854,17 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
@@ -3875,7 +3875,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>123</v>
       </c>
@@ -3886,7 +3886,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>126</v>
       </c>
@@ -3897,7 +3897,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>129</v>
       </c>
@@ -3908,7 +3908,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>132</v>
       </c>
@@ -3919,7 +3919,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>135</v>
       </c>
@@ -3930,7 +3930,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>138</v>
       </c>
@@ -3941,7 +3941,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>141</v>
       </c>
@@ -3952,7 +3952,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>142</v>
       </c>
@@ -3963,7 +3963,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>145</v>
       </c>
@@ -3974,7 +3974,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>148</v>
       </c>
@@ -3985,7 +3985,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>151</v>
       </c>
@@ -3996,7 +3996,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>154</v>
       </c>
@@ -4007,7 +4007,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>157</v>
       </c>
@@ -4018,7 +4018,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>160</v>
       </c>
@@ -4039,17 +4039,17 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
@@ -4060,7 +4060,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -4071,7 +4071,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>87</v>
       </c>
@@ -4082,7 +4082,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>114</v>
       </c>
@@ -4093,7 +4093,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>241</v>
       </c>
@@ -4104,7 +4104,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>244</v>
       </c>
@@ -4115,7 +4115,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>247</v>
       </c>
@@ -4126,7 +4126,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>250</v>
       </c>
@@ -4137,7 +4137,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>253</v>
       </c>
@@ -4148,7 +4148,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>256</v>
       </c>
@@ -4159,7 +4159,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>313</v>
       </c>
@@ -4180,16 +4180,16 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
@@ -4200,7 +4200,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>259</v>
       </c>
@@ -4211,7 +4211,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>262</v>
       </c>
@@ -4222,7 +4222,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>265</v>
       </c>
@@ -4233,7 +4233,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>268</v>
       </c>
@@ -4244,7 +4244,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>271</v>
       </c>
@@ -4255,7 +4255,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>274</v>
       </c>
@@ -4266,7 +4266,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>277</v>
       </c>
@@ -4277,7 +4277,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>280</v>
       </c>
@@ -4289,7 +4289,7 @@
       </c>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>283</v>
       </c>
@@ -4300,7 +4300,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>286</v>
       </c>
@@ -4320,21 +4320,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F8C17F5-F1B3-4EEB-A09D-046028937F0E}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -4342,7 +4342,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -4350,7 +4350,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -4358,7 +4358,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -4366,7 +4366,7 @@
         <v>-0.3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -4374,7 +4374,7 @@
         <v>-0.6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -4382,7 +4382,7 @@
         <v>-1.1000000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -4390,7 +4390,7 @@
         <v>-1.2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -4398,7 +4398,7 @@
         <v>-2.2000000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -4406,7 +4406,7 @@
         <v>-3.3</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -4427,17 +4427,17 @@
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -4445,7 +4445,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -4453,7 +4453,7 @@
         <v>-0.8</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -4461,7 +4461,7 @@
         <v>-4.5999999999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -4469,7 +4469,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -4477,7 +4477,7 @@
         <v>-8.5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -4485,7 +4485,7 @@
         <v>-8.6999999999999993</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -4493,7 +4493,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -4501,7 +4501,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -4509,7 +4509,7 @@
         <v>-10.5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -4530,15 +4530,15 @@
       <selection activeCell="V22" sqref="V22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="26.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
         <v>14</v>
       </c>
@@ -4555,7 +4555,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -4581,7 +4581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -4607,7 +4607,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -4633,7 +4633,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -4659,7 +4659,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -4673,7 +4673,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -4687,7 +4687,7 @@
         <v>-10.5</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -4701,7 +4701,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -4715,7 +4715,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -4729,7 +4729,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -4743,12 +4743,12 @@
         <v>-0.8</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -4759,7 +4759,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -4785,14 +4785,14 @@
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
@@ -4803,7 +4803,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>166</v>
       </c>
@@ -4814,7 +4814,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>123</v>
       </c>
@@ -4825,7 +4825,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>169</v>
       </c>
@@ -4836,7 +4836,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>172</v>
       </c>
@@ -4847,7 +4847,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>175</v>
       </c>
@@ -4858,7 +4858,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>178</v>
       </c>
@@ -4869,7 +4869,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>181</v>
       </c>
@@ -4880,7 +4880,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>184</v>
       </c>
@@ -4891,7 +4891,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>187</v>
       </c>
@@ -4902,7 +4902,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>190</v>
       </c>
@@ -4913,7 +4913,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>193</v>
       </c>
@@ -4924,7 +4924,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>196</v>
       </c>
@@ -4935,7 +4935,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>208</v>
       </c>
@@ -4946,7 +4946,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>211</v>
       </c>
@@ -4957,7 +4957,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>214</v>
       </c>
@@ -4968,7 +4968,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>217</v>
       </c>
@@ -4979,7 +4979,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>220</v>
       </c>
@@ -5000,18 +5000,18 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="19.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.1640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
@@ -5022,7 +5022,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>196</v>
       </c>
@@ -5033,7 +5033,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>169</v>
       </c>
@@ -5044,7 +5044,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>228</v>
       </c>
@@ -5055,7 +5055,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>229</v>
       </c>
@@ -5066,7 +5066,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>232</v>
       </c>
@@ -5077,7 +5077,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>240</v>
       </c>
@@ -5088,7 +5088,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>235</v>
       </c>
@@ -5099,7 +5099,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>68</v>
       </c>
@@ -5110,7 +5110,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>289</v>
       </c>
@@ -5121,7 +5121,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>292</v>
       </c>
@@ -5141,18 +5141,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E335B91A-270B-4B44-9FF8-13EFF3986A47}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
@@ -5163,7 +5163,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>223</v>
       </c>
@@ -5174,7 +5174,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>148</v>
       </c>
@@ -5185,7 +5185,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>163</v>
       </c>
@@ -5196,7 +5196,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>199</v>
       </c>
@@ -5207,7 +5207,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>202</v>
       </c>
@@ -5218,7 +5218,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>205</v>
       </c>
@@ -5229,7 +5229,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>295</v>
       </c>
@@ -5240,7 +5240,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>298</v>
       </c>
@@ -5251,7 +5251,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>301</v>
       </c>
@@ -5262,7 +5262,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>304</v>
       </c>
@@ -5273,7 +5273,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>310</v>
       </c>
@@ -5284,7 +5284,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>307</v>
       </c>
@@ -5308,14 +5308,14 @@
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
@@ -5326,7 +5326,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -5337,7 +5337,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -5348,7 +5348,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -5359,7 +5359,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -5370,7 +5370,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -5381,7 +5381,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -5392,7 +5392,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>41</v>
       </c>
@@ -5403,7 +5403,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -5414,7 +5414,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -5425,7 +5425,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -5436,7 +5436,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>53</v>
       </c>
@@ -5447,7 +5447,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -5458,7 +5458,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>59</v>
       </c>
@@ -5469,7 +5469,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>62</v>
       </c>
@@ -5480,7 +5480,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>65</v>
       </c>
@@ -5491,7 +5491,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>71</v>
       </c>
@@ -5502,7 +5502,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>74</v>
       </c>
@@ -5513,7 +5513,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>77</v>
       </c>
@@ -5524,7 +5524,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>80</v>
       </c>
@@ -5543,20 +5543,20 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD634B01-A1A0-4C1A-9F74-9C307E86FE41}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView zoomScale="159" zoomScaleNormal="304" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
@@ -5567,7 +5567,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>99</v>
       </c>
@@ -5578,7 +5578,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>102</v>
       </c>
@@ -5589,7 +5589,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>105</v>
       </c>
@@ -5600,7 +5600,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>108</v>
       </c>
@@ -5611,7 +5611,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>111</v>
       </c>
@@ -5622,7 +5622,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>117</v>
       </c>
@@ -5633,7 +5633,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>120</v>
       </c>
@@ -5644,7 +5644,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>84</v>
       </c>
@@ -5655,7 +5655,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>90</v>
       </c>
@@ -5666,7 +5666,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>93</v>
       </c>
@@ -5675,17 +5675,6 @@
       </c>
       <c r="C11" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>90</v>
-      </c>
-      <c r="B12" t="s">
-        <v>91</v>
-      </c>
-      <c r="C12" t="s">
-        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -5955,8 +5944,16 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6EFEB780-1A22-4CC1-8525-2972EBF6187E}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="0c2c417d-3ca9-4133-8d41-136ced1690eb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="5668a3bb-2120-40c0-b744-d1cc28798bc9"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Changes to code of web app
</commit_message>
<xml_diff>
--- a/colour-theory/colour-palettes/colours.xlsx
+++ b/colour-theory/colour-palettes/colours.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/dr19500_bristol_ac_uk/Documents/Project 2020/colour-theory/colour-palettes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="144" documentId="8_{7C6CD7C7-0BCB-4184-B93E-C2276493D1ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0A9988E4-A495-3440-B1CC-841BDFFD4E34}"/>
+  <xr:revisionPtr revIDLastSave="152" documentId="8_{7C6CD7C7-0BCB-4184-B93E-C2276493D1ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B7CD4961-7461-46E8-BFB7-8EE7B4A60AD2}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{E8E95DA0-770C-4812-975B-CF66929D1793}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="120" windowWidth="14500" windowHeight="9460" firstSheet="2" activeTab="7" xr2:uid="{E8E95DA0-770C-4812-975B-CF66929D1793}"/>
   </bookViews>
   <sheets>
     <sheet name="Pleasure" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="318">
   <si>
     <t>Blue</t>
   </si>
@@ -992,13 +992,19 @@
   </si>
   <si>
     <t>rgb(183,132,167)</t>
+  </si>
+  <si>
+    <t>http://www.rinkydinkelectronics.com/calc_rgb565.php</t>
+  </si>
+  <si>
+    <t>RGB 565</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1036,6 +1042,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1054,18 +1075,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1084,7 +1108,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1682,7 +1706,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3750,13 +3774,13 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -3764,7 +3788,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -3772,7 +3796,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -3780,7 +3804,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -3788,7 +3812,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -3796,7 +3820,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -3804,7 +3828,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -3812,7 +3836,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -3820,7 +3844,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -3828,7 +3852,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -3836,7 +3860,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -3857,14 +3881,14 @@
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
@@ -3875,7 +3899,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>123</v>
       </c>
@@ -3886,7 +3910,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>126</v>
       </c>
@@ -3897,7 +3921,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>129</v>
       </c>
@@ -3908,7 +3932,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>132</v>
       </c>
@@ -3919,7 +3943,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>135</v>
       </c>
@@ -3930,7 +3954,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>138</v>
       </c>
@@ -3941,7 +3965,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>141</v>
       </c>
@@ -3952,7 +3976,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>142</v>
       </c>
@@ -3963,7 +3987,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>145</v>
       </c>
@@ -3974,7 +3998,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>148</v>
       </c>
@@ -3985,7 +4009,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>151</v>
       </c>
@@ -3996,7 +4020,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>154</v>
       </c>
@@ -4007,7 +4031,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>157</v>
       </c>
@@ -4018,7 +4042,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>160</v>
       </c>
@@ -4042,14 +4066,14 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
@@ -4060,7 +4084,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -4071,7 +4095,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>87</v>
       </c>
@@ -4082,7 +4106,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>114</v>
       </c>
@@ -4093,7 +4117,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>241</v>
       </c>
@@ -4104,7 +4128,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>244</v>
       </c>
@@ -4115,7 +4139,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>247</v>
       </c>
@@ -4126,7 +4150,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>250</v>
       </c>
@@ -4137,7 +4161,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>253</v>
       </c>
@@ -4148,7 +4172,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>256</v>
       </c>
@@ -4159,7 +4183,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>313</v>
       </c>
@@ -4183,13 +4207,13 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
@@ -4200,7 +4224,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>259</v>
       </c>
@@ -4211,7 +4235,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>262</v>
       </c>
@@ -4222,7 +4246,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>265</v>
       </c>
@@ -4233,7 +4257,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>268</v>
       </c>
@@ -4244,7 +4268,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>271</v>
       </c>
@@ -4255,7 +4279,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>274</v>
       </c>
@@ -4266,7 +4290,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>277</v>
       </c>
@@ -4277,7 +4301,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>280</v>
       </c>
@@ -4289,7 +4313,7 @@
       </c>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>283</v>
       </c>
@@ -4300,7 +4324,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>286</v>
       </c>
@@ -4320,21 +4344,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F8C17F5-F1B3-4EEB-A09D-046028937F0E}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -4342,7 +4366,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -4350,7 +4374,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -4358,7 +4382,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -4366,7 +4390,7 @@
         <v>-0.3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -4374,7 +4398,7 @@
         <v>-0.6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -4382,7 +4406,7 @@
         <v>-1.1000000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -4390,7 +4414,7 @@
         <v>-1.2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -4398,7 +4422,7 @@
         <v>-2.2000000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -4406,7 +4430,7 @@
         <v>-3.3</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -4427,17 +4451,17 @@
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -4445,7 +4469,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -4453,7 +4477,7 @@
         <v>-0.8</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -4461,7 +4485,7 @@
         <v>-4.5999999999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -4469,7 +4493,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -4477,7 +4501,7 @@
         <v>-8.5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -4485,7 +4509,7 @@
         <v>-8.6999999999999993</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -4493,7 +4517,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -4501,7 +4525,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -4509,7 +4533,7 @@
         <v>-10.5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -4530,15 +4554,15 @@
       <selection activeCell="V22" sqref="V22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="26.81640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="26.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
         <v>14</v>
       </c>
@@ -4555,7 +4579,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -4581,7 +4605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -4607,7 +4631,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -4633,7 +4657,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -4659,7 +4683,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -4673,7 +4697,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -4687,7 +4711,7 @@
         <v>-10.5</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -4701,7 +4725,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -4715,7 +4739,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -4729,7 +4753,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -4743,12 +4767,12 @@
         <v>-0.8</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -4759,7 +4783,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -4785,14 +4809,14 @@
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
@@ -4803,7 +4827,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>166</v>
       </c>
@@ -4814,7 +4838,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>123</v>
       </c>
@@ -4825,7 +4849,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>169</v>
       </c>
@@ -4836,7 +4860,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>172</v>
       </c>
@@ -4847,7 +4871,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>175</v>
       </c>
@@ -4858,7 +4882,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>178</v>
       </c>
@@ -4869,7 +4893,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>181</v>
       </c>
@@ -4880,7 +4904,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>184</v>
       </c>
@@ -4891,7 +4915,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>187</v>
       </c>
@@ -4902,7 +4926,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>190</v>
       </c>
@@ -4913,7 +4937,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>193</v>
       </c>
@@ -4924,7 +4948,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>196</v>
       </c>
@@ -4935,7 +4959,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>208</v>
       </c>
@@ -4946,7 +4970,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>211</v>
       </c>
@@ -4957,7 +4981,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>214</v>
       </c>
@@ -4968,7 +4992,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>217</v>
       </c>
@@ -4979,7 +5003,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>220</v>
       </c>
@@ -5003,15 +5027,15 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.1640625" style="3"/>
+    <col min="1" max="1" width="19.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
@@ -5022,7 +5046,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>196</v>
       </c>
@@ -5033,7 +5057,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>169</v>
       </c>
@@ -5044,7 +5068,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>228</v>
       </c>
@@ -5055,7 +5079,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>229</v>
       </c>
@@ -5066,7 +5090,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>232</v>
       </c>
@@ -5077,7 +5101,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>240</v>
       </c>
@@ -5088,7 +5112,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>235</v>
       </c>
@@ -5099,7 +5123,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>68</v>
       </c>
@@ -5110,7 +5134,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>289</v>
       </c>
@@ -5121,7 +5145,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>292</v>
       </c>
@@ -5145,14 +5169,14 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
@@ -5163,7 +5187,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>223</v>
       </c>
@@ -5174,7 +5198,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>148</v>
       </c>
@@ -5185,7 +5209,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>163</v>
       </c>
@@ -5196,7 +5220,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>199</v>
       </c>
@@ -5207,7 +5231,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>202</v>
       </c>
@@ -5218,7 +5242,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>205</v>
       </c>
@@ -5229,7 +5253,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>295</v>
       </c>
@@ -5240,7 +5264,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>298</v>
       </c>
@@ -5251,7 +5275,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>301</v>
       </c>
@@ -5262,7 +5286,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>304</v>
       </c>
@@ -5273,7 +5297,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>310</v>
       </c>
@@ -5284,7 +5308,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>307</v>
       </c>
@@ -5302,20 +5326,20 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C48BFA2-EF61-4D34-A13A-776F3C06B7BA}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
@@ -5325,8 +5349,11 @@
       <c r="C1" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="6" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -5337,7 +5364,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -5348,7 +5375,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -5359,7 +5386,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -5370,7 +5397,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -5381,7 +5408,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -5392,7 +5419,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>41</v>
       </c>
@@ -5403,7 +5430,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -5414,7 +5441,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -5425,7 +5452,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -5436,7 +5463,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>53</v>
       </c>
@@ -5447,7 +5474,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -5458,7 +5485,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>59</v>
       </c>
@@ -5469,7 +5496,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>62</v>
       </c>
@@ -5480,7 +5507,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>65</v>
       </c>
@@ -5491,7 +5518,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>71</v>
       </c>
@@ -5502,7 +5529,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>74</v>
       </c>
@@ -5513,7 +5540,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>77</v>
       </c>
@@ -5524,7 +5551,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>80</v>
       </c>
@@ -5533,6 +5560,11 @@
       </c>
       <c r="C20" t="s">
         <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>316</v>
       </c>
     </row>
   </sheetData>
@@ -5549,14 +5581,14 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
@@ -5567,7 +5599,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>99</v>
       </c>
@@ -5578,7 +5610,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>102</v>
       </c>
@@ -5589,7 +5621,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>105</v>
       </c>
@@ -5600,7 +5632,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>108</v>
       </c>
@@ -5611,7 +5643,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>111</v>
       </c>
@@ -5622,7 +5654,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>117</v>
       </c>
@@ -5633,7 +5665,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>120</v>
       </c>
@@ -5644,7 +5676,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>84</v>
       </c>
@@ -5655,7 +5687,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>90</v>
       </c>
@@ -5666,7 +5698,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>93</v>
       </c>
@@ -5683,6 +5715,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010013BE5E99095590498FB9FAFDD56D1F68" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9ea8a5d2e5e752c43221f8cce0adf310">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0c2c417d-3ca9-4133-8d41-136ced1690eb" xmlns:ns4="5668a3bb-2120-40c0-b744-d1cc28798bc9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d1273cc37b07eb902f37205f1c9ffb1a" ns3:_="" ns4:_="">
     <xsd:import namespace="0c2c417d-3ca9-4133-8d41-136ced1690eb"/>
@@ -5899,15 +5940,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -5915,6 +5947,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B663F316-0AE1-4C04-A598-046FC969F8A3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6837176B-ADEA-41B0-BB20-E7569836195D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5929,14 +5969,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B663F316-0AE1-4C04-A598-046FC969F8A3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>